<commit_message>
Update the tracker with static remove function and upload new outputs
</commit_message>
<xml_diff>
--- a/Yizhi_pred_outputs/Yizhi_pred_outputs.xlsx
+++ b/Yizhi_pred_outputs/Yizhi_pred_outputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="28770" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
   <si>
     <t>model</t>
   </si>
@@ -238,6 +238,138 @@
   </si>
   <si>
     <t>yolox_m</t>
+  </si>
+  <si>
+    <t>pred.txt</t>
+  </si>
+  <si>
+    <r>
+      <t>drop_each_frame=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_8_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_29_11.txt</t>
+  </si>
+  <si>
+    <r>
+      <t>drop_each_frame=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_7_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_36_36.txt</t>
+  </si>
+  <si>
+    <r>
+      <t>drop_each_frame=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_6_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_25_52.txt</t>
+  </si>
+  <si>
+    <r>
+      <t>drop_each_frame=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_5_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_34_42.txt</t>
+  </si>
+  <si>
+    <r>
+      <t>drop_each_frame=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_4_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_22_50.txt</t>
+  </si>
+  <si>
+    <r>
+      <t>drop_each_frame=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF098156"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_3_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_32_02.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_2_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_19_33.txt</t>
+  </si>
+  <si>
+    <t>yolox_l</t>
   </si>
 </sst>
 </file>
@@ -250,13 +382,40 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.5"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -717,10 +876,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -729,137 +888,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -869,7 +1028,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1220,10 +1394,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1256,7 +1430,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:5">
+    <row r="2" s="1" customFormat="1" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1266,14 +1440,17 @@
       <c r="C2" s="3">
         <v>49.542</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:5">
+      <c r="F2" s="4">
+        <v>0.7122</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -1287,8 +1464,11 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:5">
+      <c r="F3" s="5">
+        <v>0.7027</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:6">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
@@ -1302,8 +1482,11 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" ht="14.25" spans="1:5">
+      <c r="F4" s="5">
+        <v>0.6975</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:6">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>16</v>
@@ -1317,8 +1500,11 @@
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" ht="14.25" spans="1:5">
+      <c r="F5" s="4">
+        <v>0.6957</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" spans="1:6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>19</v>
@@ -1332,8 +1518,11 @@
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" ht="14.25" spans="1:5">
+      <c r="F6" s="5">
+        <v>0.697</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="1:6">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -1347,8 +1536,11 @@
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" spans="1:5">
+      <c r="F7" s="5">
+        <v>0.6852</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" spans="1:6">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>25</v>
@@ -1356,14 +1548,17 @@
       <c r="C8" s="3">
         <v>62.581</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" spans="1:5">
+      <c r="F8" s="5">
+        <v>0.6729</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" spans="1:6">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>28</v>
@@ -1371,25 +1566,220 @@
       <c r="C9" s="3">
         <v>73.127</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="F9" s="4">
+        <v>0.6425</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>22.495</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.7687</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" spans="1:6">
       <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="6">
+        <v>25.633</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.7641</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" spans="1:6">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6">
+        <v>26.133</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.7549</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" spans="1:6">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6">
+        <v>26.618</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.7537</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" spans="1:6">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="6">
+        <v>27.549</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.7468</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" spans="1:6">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6">
+        <v>29.003</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.7331</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:6">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7">
+        <v>32.189</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.7185</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:6">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7">
+        <v>40.517</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.6814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" ht="14.25" spans="1:6">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" ht="14.25" spans="1:6">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" ht="14.25" spans="1:2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" spans="1:2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" spans="1:2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" spans="1:2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" spans="1:2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="A18:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
debug the static remove funtion
</commit_message>
<xml_diff>
--- a/Yizhi_pred_outputs/Yizhi_pred_outputs.xlsx
+++ b/Yizhi_pred_outputs/Yizhi_pred_outputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28770" windowHeight="12330"/>
+    <workbookView windowWidth="28770" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
   <si>
     <t>model</t>
   </si>
   <si>
     <t>parameter</t>
+  </si>
+  <si>
+    <t>Remaining frames</t>
   </si>
   <si>
     <t>FPS</t>
@@ -371,6 +374,81 @@
   <si>
     <t>yolox_l</t>
   </si>
+  <si>
+    <t>2023_01_22_08_46_50.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_8_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_08_33_46.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_7_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_46_39.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_6_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_49_58.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_5_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_53_07.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_4_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_55_31.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_3_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_59_55.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_2_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_08_09_37.txt</t>
+  </si>
+  <si>
+    <t>bytetrack_s_mot17</t>
+  </si>
+  <si>
+    <t>d=8</t>
+  </si>
+  <si>
+    <t>d=7</t>
+  </si>
+  <si>
+    <t>d=6</t>
+  </si>
+  <si>
+    <t>d=5</t>
+  </si>
+  <si>
+    <t>d=4</t>
+  </si>
+  <si>
+    <t>d=3</t>
+  </si>
+  <si>
+    <t>d=2</t>
+  </si>
+  <si>
+    <t>bytetrack_m_mot17</t>
+  </si>
+  <si>
+    <t>bytetrack_l_mot17</t>
+  </si>
 </sst>
 </file>
 
@@ -382,13 +460,32 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -411,13 +508,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.5"/>
-      <color rgb="FF212121"/>
-      <name val="Courier New"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -762,12 +852,32 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -876,10 +986,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -888,163 +998,190 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1394,386 +1531,561 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="19.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="9" style="13"/>
+    <col min="2" max="2" width="19.25" style="13" customWidth="1"/>
+    <col min="3" max="3" width="17" style="13" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="38.25" style="13" customWidth="1"/>
+    <col min="6" max="6" width="29.375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="12.625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" s="13" customFormat="1" spans="1:7">
+      <c r="A2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="13">
+        <v>654</v>
+      </c>
+      <c r="D2" s="15">
         <v>49.542</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0.7122</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:7">
+      <c r="A3" s="14"/>
+      <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="16">
+        <v>573</v>
+      </c>
+      <c r="D3" s="15">
+        <v>50.938</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="13">
+        <v>0.7027</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:7">
+      <c r="A4" s="14"/>
+      <c r="B4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="16">
+        <v>560</v>
+      </c>
+      <c r="D4" s="15">
+        <v>51.545</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="13">
+        <v>0.6975</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:7">
+      <c r="A5" s="14"/>
+      <c r="B5" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="16">
+        <v>545</v>
+      </c>
+      <c r="D5" s="15">
+        <v>51.319</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0.6957</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" spans="1:7">
+      <c r="A6" s="14"/>
+      <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="16">
+        <v>523</v>
+      </c>
+      <c r="D6" s="15">
+        <v>53.706</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0.697</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" spans="1:7">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="16">
+        <v>491</v>
+      </c>
+      <c r="D7" s="15">
+        <v>59.13</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.6852</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" spans="1:7">
+      <c r="A8" s="14"/>
+      <c r="B8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="16">
+        <v>436</v>
+      </c>
+      <c r="D8" s="15">
+        <v>62.581</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="13">
+        <v>0.6729</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" spans="1:8">
+      <c r="A9" s="14"/>
+      <c r="B9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="13">
+        <v>327</v>
+      </c>
+      <c r="D9" s="15">
+        <v>73.127</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0.6425</v>
+      </c>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C10" s="13">
+        <v>654</v>
+      </c>
+      <c r="D10" s="13">
+        <v>22.495</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4">
-        <v>0.7122</v>
-      </c>
-    </row>
-    <row r="3" ht="14.25" spans="1:6">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3">
-        <v>50.938</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="F10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.7687</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" spans="1:7">
+      <c r="A11" s="14"/>
+      <c r="B11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="16">
+        <v>573</v>
+      </c>
+      <c r="D11" s="13">
+        <v>25.633</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="13">
+        <v>0.7641</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" spans="1:7">
+      <c r="A12" s="14"/>
+      <c r="B12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="16">
+        <v>560</v>
+      </c>
+      <c r="D12" s="13">
+        <v>26.133</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="13">
+        <v>0.7549</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" spans="1:7">
+      <c r="A13" s="14"/>
+      <c r="B13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="16">
+        <v>545</v>
+      </c>
+      <c r="D13" s="13">
+        <v>26.618</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.7537</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" spans="1:7">
+      <c r="A14" s="14"/>
+      <c r="B14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="16">
+        <v>523</v>
+      </c>
+      <c r="D14" s="13">
+        <v>27.549</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.7468</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" spans="1:7">
+      <c r="A15" s="14"/>
+      <c r="B15" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="16">
+        <v>491</v>
+      </c>
+      <c r="D15" s="13">
+        <v>29.003</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.7331</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:7">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="16">
+        <v>436</v>
+      </c>
+      <c r="D16" s="15">
+        <v>32.189</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.7185</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:7">
+      <c r="A17" s="14"/>
+      <c r="B17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="13">
+        <v>327</v>
+      </c>
+      <c r="D17" s="15">
+        <v>40.517</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.6814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="13">
+        <v>654</v>
+      </c>
+      <c r="D18" s="13">
+        <v>22.19</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.7911</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" spans="1:7">
+      <c r="A19" s="14"/>
+      <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.7027</v>
-      </c>
-    </row>
-    <row r="4" ht="14.25" spans="1:6">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
-        <v>51.545</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C19" s="16">
+        <v>573</v>
+      </c>
+      <c r="D19" s="13">
+        <v>23.479</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.7793</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" spans="1:7">
+      <c r="A20" s="14"/>
+      <c r="B20" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.6975</v>
-      </c>
-    </row>
-    <row r="5" ht="14.25" spans="1:6">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3">
-        <v>51.319</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C20" s="16">
+        <v>560</v>
+      </c>
+      <c r="D20" s="13">
+        <v>24.625</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.7766</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" spans="1:7">
+      <c r="A21" s="14"/>
+      <c r="B21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.6957</v>
-      </c>
-    </row>
-    <row r="6" ht="14.25" spans="1:6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3">
-        <v>53.706</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C21" s="16">
+        <v>545</v>
+      </c>
+      <c r="D21" s="13">
+        <v>24.598</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0.7716</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" spans="1:7">
+      <c r="A22" s="14"/>
+      <c r="B22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.697</v>
-      </c>
-    </row>
-    <row r="7" ht="14.25" spans="1:6">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3">
-        <v>59.13</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C22" s="16">
+        <v>523</v>
+      </c>
+      <c r="D22" s="13">
+        <v>25.85</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.7675</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" spans="1:7">
+      <c r="A23" s="14"/>
+      <c r="B23" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.6852</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" spans="1:6">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3">
-        <v>62.581</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C23" s="16">
+        <v>491</v>
+      </c>
+      <c r="D23" s="13">
+        <v>27.369</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.7553</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" spans="1:7">
+      <c r="A24" s="14"/>
+      <c r="B24" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.6729</v>
-      </c>
-    </row>
-    <row r="9" ht="14.25" spans="1:6">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="3">
-        <v>73.127</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C24" s="16">
+        <v>436</v>
+      </c>
+      <c r="D24" s="13">
+        <v>29.934</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0.7488</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" spans="1:7">
+      <c r="A25" s="14"/>
+      <c r="B25" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.6425</v>
-      </c>
-    </row>
-    <row r="10" ht="14.25" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="6">
-        <v>22.495</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.7687</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" spans="1:6">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="6">
-        <v>25.633</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.7641</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" spans="1:6">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="6">
-        <v>26.133</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.7549</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" spans="1:6">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="6">
-        <v>26.618</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.7537</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" spans="1:6">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="6">
-        <v>27.549</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0.7468</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25" spans="1:6">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="6">
-        <v>29.003</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0.7331</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" spans="1:6">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="7">
-        <v>32.189</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0.7185</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" spans="1:6">
-      <c r="A17" s="2"/>
-      <c r="B17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="7">
-        <v>40.517</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0.6814</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" ht="14.25" spans="1:6">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="8"/>
-    </row>
-    <row r="20" ht="14.25" spans="1:6">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" ht="14.25" spans="1:2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" spans="1:2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" spans="1:2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" spans="1:2">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25" spans="1:2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="C25" s="13">
+        <v>327</v>
+      </c>
+      <c r="D25" s="15">
+        <v>36.248</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.7018</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" spans="4:5">
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1790,14 +2102,427 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A6:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" ht="14.25" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" ht="14.25" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" ht="15" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>654</v>
+      </c>
+      <c r="C8" s="7">
+        <v>49.542</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.7122</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:4">
+      <c r="A9" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="9">
+        <v>573</v>
+      </c>
+      <c r="C9" s="7">
+        <v>50.938</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.7027</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="9">
+        <v>560</v>
+      </c>
+      <c r="C10" s="7">
+        <v>51.545</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.6975</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="9">
+        <v>545</v>
+      </c>
+      <c r="C11" s="7">
+        <v>51.319</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.6957</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="9">
+        <v>523</v>
+      </c>
+      <c r="C12" s="7">
+        <v>53.706</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.697</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:4">
+      <c r="A13" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="9">
+        <v>491</v>
+      </c>
+      <c r="C13" s="7">
+        <v>59.13</v>
+      </c>
+      <c r="D13" s="6">
+        <v>0.6852</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:4">
+      <c r="A14" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="9">
+        <v>436</v>
+      </c>
+      <c r="C14" s="7">
+        <v>62.581</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.6729</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:4">
+      <c r="A15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="11">
+        <v>327</v>
+      </c>
+      <c r="C15" s="12">
+        <v>73.127</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0.6425</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:4">
+      <c r="A16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" ht="14.25" spans="1:4">
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" ht="15" spans="1:4">
+      <c r="A18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5">
+        <v>654</v>
+      </c>
+      <c r="C18" s="5">
+        <v>22.495</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.7687</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:4">
+      <c r="A19" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="6">
+        <v>573</v>
+      </c>
+      <c r="C19" s="6">
+        <v>25.633</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.7641</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:4">
+      <c r="A20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="6">
+        <v>560</v>
+      </c>
+      <c r="C20" s="6">
+        <v>26.133</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.7549</v>
+      </c>
+    </row>
+    <row r="21" ht="15" spans="1:4">
+      <c r="A21" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="6">
+        <v>545</v>
+      </c>
+      <c r="C21" s="6">
+        <v>26.618</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.7537</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:4">
+      <c r="A22" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="6">
+        <v>523</v>
+      </c>
+      <c r="C22" s="6">
+        <v>27.549</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.7468</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:4">
+      <c r="A23" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" s="6">
+        <v>491</v>
+      </c>
+      <c r="C23" s="6">
+        <v>29.003</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.7331</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:4">
+      <c r="A24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="6">
+        <v>436</v>
+      </c>
+      <c r="C24" s="7">
+        <v>32.189</v>
+      </c>
+      <c r="D24" s="6">
+        <v>0.7185</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:4">
+      <c r="A25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="11">
+        <v>327</v>
+      </c>
+      <c r="C25" s="12">
+        <v>40.517</v>
+      </c>
+      <c r="D25" s="11">
+        <v>0.6814</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" spans="1:4">
+      <c r="A26" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" ht="14.25" spans="1:4">
+      <c r="A27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" ht="15" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="6">
+        <v>654</v>
+      </c>
+      <c r="C28" s="6">
+        <v>22.19</v>
+      </c>
+      <c r="D28" s="6">
+        <v>0.7911</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:4">
+      <c r="A29" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="9">
+        <v>573</v>
+      </c>
+      <c r="C29" s="6">
+        <v>23.479</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.7793</v>
+      </c>
+    </row>
+    <row r="30" ht="15" spans="1:4">
+      <c r="A30" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="9">
+        <v>560</v>
+      </c>
+      <c r="C30" s="6">
+        <v>24.625</v>
+      </c>
+      <c r="D30" s="6">
+        <v>0.7766</v>
+      </c>
+    </row>
+    <row r="31" ht="15" spans="1:4">
+      <c r="A31" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" s="9">
+        <v>545</v>
+      </c>
+      <c r="C31" s="6">
+        <v>24.598</v>
+      </c>
+      <c r="D31" s="6">
+        <v>0.7716</v>
+      </c>
+    </row>
+    <row r="32" ht="15" spans="1:4">
+      <c r="A32" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="9">
+        <v>523</v>
+      </c>
+      <c r="C32" s="6">
+        <v>25.85</v>
+      </c>
+      <c r="D32" s="6">
+        <v>0.7675</v>
+      </c>
+    </row>
+    <row r="33" ht="15" spans="1:4">
+      <c r="A33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="9">
+        <v>491</v>
+      </c>
+      <c r="C33" s="6">
+        <v>27.369</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.7553</v>
+      </c>
+    </row>
+    <row r="34" ht="15" spans="1:4">
+      <c r="A34" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="9">
+        <v>436</v>
+      </c>
+      <c r="C34" s="6">
+        <v>29.934</v>
+      </c>
+      <c r="D34" s="6">
+        <v>0.7488</v>
+      </c>
+    </row>
+    <row r="35" ht="15" spans="1:4">
+      <c r="A35" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="11">
+        <v>327</v>
+      </c>
+      <c r="C35" s="12">
+        <v>36.248</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0.7018</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A26:D26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Debug the static remove function, upload a visualization function
</commit_message>
<xml_diff>
--- a/Yizhi_pred_outputs/Yizhi_pred_outputs.xlsx
+++ b/Yizhi_pred_outputs/Yizhi_pred_outputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28770" windowHeight="12330" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
   <si>
     <t>model</t>
   </si>
@@ -246,8 +246,107 @@
     <t>pred.txt</t>
   </si>
   <si>
+    <t>gt_processed_drop_each_frame_8_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_29_11.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_7_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_36_36.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_6_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_25_52.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_5_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_34_42.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_4_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_22_50.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_3_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_32_02.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_2_m.txt</t>
+  </si>
+  <si>
+    <t>2023_01_21_17_19_33.txt</t>
+  </si>
+  <si>
+    <t>yolox_l</t>
+  </si>
+  <si>
+    <t>2023_01_22_08_46_50.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_8_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_08_33_46.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_7_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_46_39.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_6_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_49_58.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_5_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_53_07.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_4_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_55_31.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_3_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_07_59_55.txt</t>
+  </si>
+  <si>
+    <t>gt_processed_drop_each_frame_2_l.txt</t>
+  </si>
+  <si>
+    <t>2023_01_22_08_09_37.txt</t>
+  </si>
+  <si>
+    <t>Did not save</t>
+  </si>
+  <si>
     <r>
-      <t>drop_each_frame=</t>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sta_thres=</t>
     </r>
     <r>
       <rPr>
@@ -256,18 +355,18 @@
         <rFont val="Courier New"/>
         <charset val="134"/>
       </rPr>
-      <t>8</t>
+      <t>0.1</t>
     </r>
   </si>
   <si>
-    <t>gt_processed_drop_each_frame_8_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_29_11.txt</t>
-  </si>
-  <si>
     <r>
-      <t>drop_each_frame=</t>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sta_thres=</t>
     </r>
     <r>
       <rPr>
@@ -276,18 +375,18 @@
         <rFont val="Courier New"/>
         <charset val="134"/>
       </rPr>
-      <t>7</t>
+      <t>0.2</t>
     </r>
   </si>
   <si>
-    <t>gt_processed_drop_each_frame_7_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_36_36.txt</t>
-  </si>
-  <si>
     <r>
-      <t>drop_each_frame=</t>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sta_thres=</t>
     </r>
     <r>
       <rPr>
@@ -296,18 +395,18 @@
         <rFont val="Courier New"/>
         <charset val="134"/>
       </rPr>
-      <t>6</t>
+      <t>0.3</t>
     </r>
   </si>
   <si>
-    <t>gt_processed_drop_each_frame_6_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_25_52.txt</t>
-  </si>
-  <si>
     <r>
-      <t>drop_each_frame=</t>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sta_thres=</t>
     </r>
     <r>
       <rPr>
@@ -316,18 +415,18 @@
         <rFont val="Courier New"/>
         <charset val="134"/>
       </rPr>
-      <t>5</t>
+      <t>0.4</t>
     </r>
   </si>
   <si>
-    <t>gt_processed_drop_each_frame_5_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_34_42.txt</t>
-  </si>
-  <si>
     <r>
-      <t>drop_each_frame=</t>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <charset val="134"/>
+      </rPr>
+      <t>sta_thres=</t>
     </r>
     <r>
       <rPr>
@@ -336,90 +435,10 @@
         <rFont val="Courier New"/>
         <charset val="134"/>
       </rPr>
-      <t>4</t>
+      <t>0.5</t>
     </r>
   </si>
   <si>
-    <t>gt_processed_drop_each_frame_4_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_22_50.txt</t>
-  </si>
-  <si>
-    <r>
-      <t>drop_each_frame=</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color rgb="FF098156"/>
-        <rFont val="Courier New"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_3_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_32_02.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_2_m.txt</t>
-  </si>
-  <si>
-    <t>2023_01_21_17_19_33.txt</t>
-  </si>
-  <si>
-    <t>yolox_l</t>
-  </si>
-  <si>
-    <t>2023_01_22_08_46_50.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_8_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_08_33_46.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_7_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_07_46_39.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_6_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_07_49_58.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_5_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_07_53_07.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_4_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_07_55_31.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_3_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_07_59_55.txt</t>
-  </si>
-  <si>
-    <t>gt_processed_drop_each_frame_2_l.txt</t>
-  </si>
-  <si>
-    <t>2023_01_22_08_09_37.txt</t>
-  </si>
-  <si>
     <t>bytetrack_s_mot17</t>
   </si>
   <si>
@@ -448,6 +467,21 @@
   </si>
   <si>
     <t>bytetrack_l_mot17</t>
+  </si>
+  <si>
+    <t>s=0.1</t>
+  </si>
+  <si>
+    <t>s=0.2</t>
+  </si>
+  <si>
+    <t>s=0.3</t>
+  </si>
+  <si>
+    <t>s=0.4</t>
+  </si>
+  <si>
+    <t>s=0.5</t>
   </si>
 </sst>
 </file>
@@ -462,6 +496,14 @@
   </numFmts>
   <fonts count="27">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -486,14 +528,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -1128,60 +1162,48 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1531,567 +1553,857 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9" style="13"/>
-    <col min="2" max="2" width="19.25" style="13" customWidth="1"/>
-    <col min="3" max="3" width="17" style="13" customWidth="1"/>
-    <col min="4" max="4" width="12.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="38.25" style="13" customWidth="1"/>
-    <col min="6" max="6" width="29.375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="9" style="2"/>
+    <col min="2" max="2" width="19.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.25" style="2" customWidth="1"/>
+    <col min="6" max="6" width="29.375" style="2" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="12.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" s="13" customFormat="1" spans="1:7">
-      <c r="A2" s="14" t="s">
+    <row r="2" s="2" customFormat="1" spans="1:7">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="2">
         <v>654</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="10">
         <v>49.542</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="2">
         <v>0.7122</v>
       </c>
     </row>
     <row r="3" ht="14.25" spans="1:7">
-      <c r="A3" s="14"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="11">
         <v>573</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="10">
         <v>50.938</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="2">
         <v>0.7027</v>
       </c>
     </row>
     <row r="4" ht="14.25" spans="1:7">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="11">
         <v>560</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="10">
         <v>51.545</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="2">
         <v>0.6975</v>
       </c>
     </row>
-    <row r="5" ht="14.25" spans="1:7">
-      <c r="A5" s="14"/>
-      <c r="B5" s="13" t="s">
+    <row r="5" ht="14.25" spans="1:9">
+      <c r="A5" s="8"/>
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="11">
         <v>545</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="10">
         <v>51.319</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="2">
         <v>0.6957</v>
       </c>
-    </row>
-    <row r="6" ht="14.25" spans="1:7">
-      <c r="A6" s="14"/>
-      <c r="B6" s="13" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" ht="14.25" spans="1:9">
+      <c r="A6" s="8"/>
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="11">
         <v>523</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="10">
         <v>53.706</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="2">
         <v>0.697</v>
       </c>
-    </row>
-    <row r="7" ht="14.25" spans="1:7">
-      <c r="A7" s="14"/>
-      <c r="B7" s="13" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" ht="14.25" spans="1:9">
+      <c r="A7" s="8"/>
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="11">
         <v>491</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="10">
         <v>59.13</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="2">
         <v>0.6852</v>
       </c>
-    </row>
-    <row r="8" ht="14.25" spans="1:7">
-      <c r="A8" s="14"/>
-      <c r="B8" s="13" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" ht="14.25" spans="1:9">
+      <c r="A8" s="8"/>
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="11">
         <v>436</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="10">
         <v>62.581</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="2">
         <v>0.6729</v>
       </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" ht="14.25" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="2">
         <v>327</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="10">
         <v>73.127</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="2">
         <v>0.6425</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="2">
         <v>654</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="2">
         <v>22.495</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="2">
         <v>0.7687</v>
       </c>
     </row>
     <row r="11" ht="14.25" spans="1:7">
-      <c r="A11" s="14"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="11">
+        <v>573</v>
+      </c>
+      <c r="D11" s="2">
+        <v>25.633</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="16">
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.7641</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25" spans="1:7">
+      <c r="A12" s="8"/>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11">
+        <v>560</v>
+      </c>
+      <c r="D12" s="2">
+        <v>26.133</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.7549</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25" spans="1:7">
+      <c r="A13" s="8"/>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="11">
+        <v>545</v>
+      </c>
+      <c r="D13" s="2">
+        <v>26.618</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0.7537</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" spans="1:7">
+      <c r="A14" s="8"/>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="11">
+        <v>523</v>
+      </c>
+      <c r="D14" s="2">
+        <v>27.549</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.7468</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" spans="1:7">
+      <c r="A15" s="8"/>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="11">
+        <v>491</v>
+      </c>
+      <c r="D15" s="2">
+        <v>29.003</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.7331</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:7">
+      <c r="A16" s="8"/>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="11">
+        <v>436</v>
+      </c>
+      <c r="D16" s="10">
+        <v>32.189</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.7185</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:7">
+      <c r="A17" s="8"/>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2">
+        <v>327</v>
+      </c>
+      <c r="D17" s="10">
+        <v>40.517</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.6814</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2">
+        <v>654</v>
+      </c>
+      <c r="D18" s="2">
+        <v>22.19</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.7911</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" spans="1:7">
+      <c r="A19" s="8"/>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="11">
         <v>573</v>
       </c>
-      <c r="D11" s="13">
-        <v>25.633</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0.7641</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" spans="1:7">
-      <c r="A12" s="14"/>
-      <c r="B12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="16">
+      <c r="D19" s="2">
+        <v>23.479</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0.7793</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" spans="1:7">
+      <c r="A20" s="8"/>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="11">
         <v>560</v>
       </c>
-      <c r="D12" s="13">
-        <v>26.133</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="13">
-        <v>0.7549</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" spans="1:7">
-      <c r="A13" s="14"/>
-      <c r="B13" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="16">
+      <c r="D20" s="2">
+        <v>24.625</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0.7766</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" spans="1:7">
+      <c r="A21" s="8"/>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="11">
         <v>545</v>
       </c>
-      <c r="D13" s="13">
-        <v>26.618</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.7537</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" spans="1:7">
-      <c r="A14" s="14"/>
-      <c r="B14" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="16">
+      <c r="D21" s="2">
+        <v>24.598</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.7716</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" spans="1:7">
+      <c r="A22" s="8"/>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="11">
         <v>523</v>
       </c>
-      <c r="D14" s="13">
-        <v>27.549</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.7468</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25" spans="1:7">
-      <c r="A15" s="14"/>
-      <c r="B15" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="16">
+      <c r="D22" s="2">
+        <v>25.85</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0.7675</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25" spans="1:7">
+      <c r="A23" s="8"/>
+      <c r="B23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="11">
         <v>491</v>
       </c>
-      <c r="D15" s="13">
-        <v>29.003</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="D23" s="2">
+        <v>27.369</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.7553</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" spans="1:7">
+      <c r="A24" s="8"/>
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="11">
+        <v>436</v>
+      </c>
+      <c r="D24" s="2">
+        <v>29.934</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.7488</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" spans="1:7">
+      <c r="A25" s="8"/>
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="2">
+        <v>327</v>
+      </c>
+      <c r="D25" s="10">
+        <v>36.248</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.7018</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2">
+        <v>654</v>
+      </c>
+      <c r="D26" s="10">
+        <v>49.542</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.7122</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" spans="1:7">
+      <c r="A27" s="8"/>
+      <c r="B27" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="2">
+        <v>589</v>
+      </c>
+      <c r="D27" s="10">
+        <v>52.146</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.7068</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" spans="1:7">
+      <c r="A28" s="8"/>
+      <c r="B28" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="2">
+        <v>524</v>
+      </c>
+      <c r="D28" s="10">
+        <v>56.724</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.7014</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" spans="1:7">
+      <c r="A29" s="8"/>
+      <c r="B29" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="2">
+        <v>458</v>
+      </c>
+      <c r="D29" s="10">
+        <v>61.047</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.695</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" spans="1:7">
+      <c r="A30" s="8"/>
+      <c r="B30" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2">
+        <v>393</v>
+      </c>
+      <c r="D30" s="10">
+        <v>67.099</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.6847</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" spans="1:7">
+      <c r="A31" s="8"/>
+      <c r="B31" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="2">
+        <v>327</v>
+      </c>
+      <c r="D31" s="10">
+        <v>73.766</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.6555</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="2">
+        <v>654</v>
+      </c>
+      <c r="D32" s="2">
+        <v>22.495</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.7687</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" spans="1:7">
+      <c r="A33" s="8"/>
+      <c r="B33" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="2">
+        <v>589</v>
+      </c>
+      <c r="D33" s="2">
+        <v>24.735</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.7625</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" spans="1:7">
+      <c r="A34" s="8"/>
+      <c r="B34" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="2">
+        <v>524</v>
+      </c>
+      <c r="D34" s="2">
+        <v>27.317</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" spans="1:7">
+      <c r="A35" s="8"/>
+      <c r="B35" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="2">
+        <v>458</v>
+      </c>
+      <c r="D35" s="10">
+        <v>30.434</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.7413</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" spans="1:7">
+      <c r="A36" s="8"/>
+      <c r="B36" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="2">
+        <v>393</v>
+      </c>
+      <c r="D36" s="10">
+        <v>34.303</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.7252</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" spans="1:7">
+      <c r="A37" s="8"/>
+      <c r="B37" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="2">
+        <v>327</v>
+      </c>
+      <c r="D37" s="10">
+        <v>39.285</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.7088</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="13">
-        <v>0.7331</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" spans="1:7">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="16">
-        <v>436</v>
-      </c>
-      <c r="D16" s="15">
-        <v>32.189</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="13">
-        <v>0.7185</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" spans="1:7">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="13">
+      <c r="B38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="2">
+        <v>654</v>
+      </c>
+      <c r="D38" s="2">
+        <v>22.19</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.7911</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" spans="1:7">
+      <c r="A39" s="8"/>
+      <c r="B39" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="2">
+        <v>589</v>
+      </c>
+      <c r="D39" s="2">
+        <v>22.19</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.7825</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" spans="1:7">
+      <c r="A40" s="8"/>
+      <c r="B40" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="2">
+        <v>524</v>
+      </c>
+      <c r="D40" s="2">
+        <v>24.037</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.7702</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25" spans="1:7">
+      <c r="A41" s="8"/>
+      <c r="B41" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="2">
+        <v>458</v>
+      </c>
+      <c r="D41" s="2">
+        <v>26.181</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.7617</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25" spans="1:7">
+      <c r="A42" s="8"/>
+      <c r="B42" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="2">
+        <v>393</v>
+      </c>
+      <c r="D42" s="2">
+        <v>27.732</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.7419</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25" spans="1:7">
+      <c r="A43" s="8"/>
+      <c r="B43" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="2">
         <v>327</v>
       </c>
-      <c r="D17" s="15">
-        <v>40.517</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="13">
-        <v>0.6814</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="13">
-        <v>654</v>
-      </c>
-      <c r="D18" s="13">
-        <v>22.19</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G18" s="13">
-        <v>0.7911</v>
-      </c>
-    </row>
-    <row r="19" ht="14.25" spans="1:7">
-      <c r="A19" s="14"/>
-      <c r="B19" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="16">
-        <v>573</v>
-      </c>
-      <c r="D19" s="13">
-        <v>23.479</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="13">
-        <v>0.7793</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" spans="1:7">
-      <c r="A20" s="14"/>
-      <c r="B20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="16">
-        <v>560</v>
-      </c>
-      <c r="D20" s="13">
-        <v>24.625</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="13">
-        <v>0.7766</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" spans="1:7">
-      <c r="A21" s="14"/>
-      <c r="B21" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="16">
-        <v>545</v>
-      </c>
-      <c r="D21" s="13">
-        <v>24.598</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="13">
-        <v>0.7716</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" spans="1:7">
-      <c r="A22" s="14"/>
-      <c r="B22" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="16">
-        <v>523</v>
-      </c>
-      <c r="D22" s="13">
-        <v>25.85</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="13">
-        <v>0.7675</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" spans="1:7">
-      <c r="A23" s="14"/>
-      <c r="B23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="16">
-        <v>491</v>
-      </c>
-      <c r="D23" s="13">
-        <v>27.369</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" s="13">
-        <v>0.7553</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" spans="1:7">
-      <c r="A24" s="14"/>
-      <c r="B24" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="16">
-        <v>436</v>
-      </c>
-      <c r="D24" s="13">
-        <v>29.934</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="13">
-        <v>0.7488</v>
-      </c>
-    </row>
-    <row r="25" ht="14.25" spans="1:7">
-      <c r="A25" s="14"/>
-      <c r="B25" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="13">
-        <v>327</v>
-      </c>
-      <c r="D25" s="15">
-        <v>36.248</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="13">
-        <v>0.7018</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" spans="4:5">
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
+      <c r="D43" s="10">
+        <v>31.88</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.7102</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7">
+      <c r="G44" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="7">
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="E26:F43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2102,426 +2414,426 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A6:D35"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="$A11:$XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="3" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" ht="14.25" spans="1:4">
-      <c r="A6" s="2" t="s">
+    <row r="1" ht="14.25" spans="1:4">
+      <c r="A1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" ht="14.25" spans="1:4">
-      <c r="A7" s="4" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" ht="14.25" spans="1:4">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="15" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>654</v>
+      </c>
+      <c r="C3" s="6">
+        <v>49.542</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.7122</v>
+      </c>
+    </row>
+    <row r="4" ht="15" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="9">
+        <v>573</v>
+      </c>
+      <c r="C4" s="6">
+        <v>50.938</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.7027</v>
+      </c>
+    </row>
+    <row r="5" ht="15" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="9">
+        <v>560</v>
+      </c>
+      <c r="C5" s="6">
+        <v>51.545</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.6975</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="9">
+        <v>545</v>
+      </c>
+      <c r="C6" s="6">
+        <v>51.319</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.6957</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="9">
+        <v>523</v>
+      </c>
+      <c r="C7" s="6">
+        <v>53.706</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.697</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:4">
       <c r="A8" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="9">
+        <v>491</v>
+      </c>
+      <c r="C8" s="6">
+        <v>59.13</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.6852</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:4">
+      <c r="A9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="9">
+        <v>436</v>
+      </c>
+      <c r="C9" s="6">
+        <v>62.581</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.6729</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:4">
+      <c r="A10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="7">
+        <v>327</v>
+      </c>
+      <c r="C10" s="4">
+        <v>73.127</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.6425</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" ht="14.25" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:4">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B13" s="5">
         <v>654</v>
       </c>
-      <c r="C8" s="7">
-        <v>49.542</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.7122</v>
-      </c>
-    </row>
-    <row r="9" ht="15" spans="1:4">
-      <c r="A9" s="8" t="s">
+      <c r="C13" s="5">
+        <v>22.495</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.7687</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:4">
+      <c r="A14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B14" s="5">
         <v>573</v>
       </c>
-      <c r="C9" s="7">
-        <v>50.938</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.7027</v>
-      </c>
-    </row>
-    <row r="10" ht="15" spans="1:4">
-      <c r="A10" s="8" t="s">
+      <c r="C14" s="5">
+        <v>25.633</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.7641</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:4">
+      <c r="A15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B15" s="5">
         <v>560</v>
       </c>
-      <c r="C10" s="7">
-        <v>51.545</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.6975</v>
-      </c>
-    </row>
-    <row r="11" ht="15" spans="1:4">
-      <c r="A11" s="8" t="s">
+      <c r="C15" s="5">
+        <v>26.133</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.7549</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:4">
+      <c r="A16" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B16" s="5">
         <v>545</v>
       </c>
-      <c r="C11" s="7">
-        <v>51.319</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.6957</v>
-      </c>
-    </row>
-    <row r="12" ht="15" spans="1:4">
-      <c r="A12" s="8" t="s">
+      <c r="C16" s="5">
+        <v>26.618</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.7537</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:4">
+      <c r="A17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B17" s="5">
         <v>523</v>
       </c>
-      <c r="C12" s="7">
-        <v>53.706</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0.697</v>
-      </c>
-    </row>
-    <row r="13" ht="15" spans="1:4">
-      <c r="A13" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B13" s="9">
-        <v>491</v>
-      </c>
-      <c r="C13" s="7">
-        <v>59.13</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0.6852</v>
-      </c>
-    </row>
-    <row r="14" ht="15" spans="1:4">
-      <c r="A14" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="9">
-        <v>436</v>
-      </c>
-      <c r="C14" s="7">
-        <v>62.581</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0.6729</v>
-      </c>
-    </row>
-    <row r="15" ht="15" spans="1:4">
-      <c r="A15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="11">
-        <v>327</v>
-      </c>
-      <c r="C15" s="12">
-        <v>73.127</v>
-      </c>
-      <c r="D15" s="11">
-        <v>0.6425</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" spans="1:4">
-      <c r="A16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" ht="14.25" spans="1:4">
-      <c r="A17" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
+      <c r="C17" s="5">
+        <v>27.549</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.7468</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:4">
       <c r="A18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="5">
+        <v>491</v>
+      </c>
+      <c r="C18" s="5">
+        <v>29.003</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.7331</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="5">
+        <v>436</v>
+      </c>
+      <c r="C19" s="6">
+        <v>32.189</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.7185</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:4">
+      <c r="A20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="7">
+        <v>327</v>
+      </c>
+      <c r="C20" s="4">
+        <v>40.517</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.6814</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" spans="1:4">
+      <c r="A21" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" ht="14.25" spans="1:4">
+      <c r="A22" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:4">
+      <c r="A23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B23" s="5">
         <v>654</v>
       </c>
-      <c r="C18" s="5">
-        <v>22.495</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.7687</v>
-      </c>
-    </row>
-    <row r="19" ht="15" spans="1:4">
-      <c r="A19" s="8" t="s">
+      <c r="C23" s="5">
+        <v>22.19</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.7911</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:4">
+      <c r="A24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B24" s="9">
         <v>573</v>
       </c>
-      <c r="C19" s="6">
-        <v>25.633</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0.7641</v>
-      </c>
-    </row>
-    <row r="20" ht="15" spans="1:4">
-      <c r="A20" s="8" t="s">
+      <c r="C24" s="5">
+        <v>23.479</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.7793</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:4">
+      <c r="A25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B25" s="9">
         <v>560</v>
       </c>
-      <c r="C20" s="6">
-        <v>26.133</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0.7549</v>
-      </c>
-    </row>
-    <row r="21" ht="15" spans="1:4">
-      <c r="A21" s="8" t="s">
+      <c r="C25" s="5">
+        <v>24.625</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0.7766</v>
+      </c>
+    </row>
+    <row r="26" ht="15" spans="1:4">
+      <c r="A26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B26" s="9">
         <v>545</v>
       </c>
-      <c r="C21" s="6">
-        <v>26.618</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0.7537</v>
-      </c>
-    </row>
-    <row r="22" ht="15" spans="1:4">
-      <c r="A22" s="8" t="s">
+      <c r="C26" s="5">
+        <v>24.598</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.7716</v>
+      </c>
+    </row>
+    <row r="27" ht="15" spans="1:4">
+      <c r="A27" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B27" s="9">
         <v>523</v>
       </c>
-      <c r="C22" s="6">
-        <v>27.549</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0.7468</v>
-      </c>
-    </row>
-    <row r="23" ht="15" spans="1:4">
-      <c r="A23" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="6">
-        <v>491</v>
-      </c>
-      <c r="C23" s="6">
-        <v>29.003</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0.7331</v>
-      </c>
-    </row>
-    <row r="24" ht="15" spans="1:4">
-      <c r="A24" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="6">
-        <v>436</v>
-      </c>
-      <c r="C24" s="7">
-        <v>32.189</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0.7185</v>
-      </c>
-    </row>
-    <row r="25" ht="15" spans="1:4">
-      <c r="A25" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="11">
-        <v>327</v>
-      </c>
-      <c r="C25" s="12">
-        <v>40.517</v>
-      </c>
-      <c r="D25" s="11">
-        <v>0.6814</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25" spans="1:4">
-      <c r="A26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" ht="14.25" spans="1:4">
-      <c r="A27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>6</v>
+      <c r="C27" s="5">
+        <v>25.85</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.7675</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:4">
       <c r="A28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="6">
-        <v>654</v>
-      </c>
-      <c r="C28" s="6">
-        <v>22.19</v>
-      </c>
-      <c r="D28" s="6">
-        <v>0.7911</v>
+        <v>75</v>
+      </c>
+      <c r="B28" s="9">
+        <v>491</v>
+      </c>
+      <c r="C28" s="5">
+        <v>27.369</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0.7553</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:4">
-      <c r="A29" s="8" t="s">
-        <v>71</v>
+      <c r="A29" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="B29" s="9">
-        <v>573</v>
-      </c>
-      <c r="C29" s="6">
-        <v>23.479</v>
-      </c>
-      <c r="D29" s="6">
-        <v>0.7793</v>
+        <v>436</v>
+      </c>
+      <c r="C29" s="5">
+        <v>29.934</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.7488</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:4">
-      <c r="A30" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="9">
-        <v>560</v>
-      </c>
-      <c r="C30" s="6">
-        <v>24.625</v>
-      </c>
-      <c r="D30" s="6">
-        <v>0.7766</v>
-      </c>
-    </row>
-    <row r="31" ht="15" spans="1:4">
-      <c r="A31" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="9">
-        <v>545</v>
-      </c>
-      <c r="C31" s="6">
-        <v>24.598</v>
-      </c>
-      <c r="D31" s="6">
-        <v>0.7716</v>
-      </c>
-    </row>
-    <row r="32" ht="15" spans="1:4">
-      <c r="A32" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B32" s="9">
-        <v>523</v>
-      </c>
-      <c r="C32" s="6">
-        <v>25.85</v>
-      </c>
-      <c r="D32" s="6">
-        <v>0.7675</v>
-      </c>
-    </row>
-    <row r="33" ht="15" spans="1:4">
-      <c r="A33" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" s="9">
-        <v>491</v>
-      </c>
-      <c r="C33" s="6">
-        <v>27.369</v>
-      </c>
-      <c r="D33" s="6">
-        <v>0.7553</v>
-      </c>
-    </row>
-    <row r="34" ht="15" spans="1:4">
-      <c r="A34" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="9">
-        <v>436</v>
-      </c>
-      <c r="C34" s="6">
-        <v>29.934</v>
-      </c>
-      <c r="D34" s="6">
-        <v>0.7488</v>
-      </c>
-    </row>
-    <row r="35" ht="15" spans="1:4">
-      <c r="A35" s="10" t="s">
+      <c r="A30" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B30" s="7">
         <v>327</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C30" s="4">
         <v>36.248</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D30" s="7">
         <v>0.7018</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2532,14 +2844,352 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A17" sqref="A17:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="4" width="16.625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" spans="1:4">
+      <c r="A1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" s="1" customFormat="1" ht="14.25" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="15" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>654</v>
+      </c>
+      <c r="C3" s="6">
+        <v>49.542</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.7122</v>
+      </c>
+    </row>
+    <row r="4" ht="15" spans="1:4">
+      <c r="A4" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="5">
+        <v>589</v>
+      </c>
+      <c r="C4" s="6">
+        <v>52.146</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.7068</v>
+      </c>
+    </row>
+    <row r="5" ht="15" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="5">
+        <v>524</v>
+      </c>
+      <c r="C5" s="6">
+        <v>56.724</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.7014</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:4">
+      <c r="A6" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="5">
+        <v>458</v>
+      </c>
+      <c r="C6" s="6">
+        <v>61.047</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.695</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:4">
+      <c r="A7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="5">
+        <v>393</v>
+      </c>
+      <c r="C7" s="6">
+        <v>67.099</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.6847</v>
+      </c>
+    </row>
+    <row r="8" ht="15" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="5">
+        <v>327</v>
+      </c>
+      <c r="C8" s="6">
+        <v>73.766</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.6555</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" ht="14.25" spans="1:4">
+      <c r="A10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="1:4">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>654</v>
+      </c>
+      <c r="C11" s="5">
+        <v>22.495</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.7687</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="1:4">
+      <c r="A12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="5">
+        <v>589</v>
+      </c>
+      <c r="C12" s="5">
+        <v>24.735</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.7625</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:4">
+      <c r="A13" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="5">
+        <v>524</v>
+      </c>
+      <c r="C13" s="5">
+        <v>27.317</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:4">
+      <c r="A14" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="5">
+        <v>458</v>
+      </c>
+      <c r="C14" s="6">
+        <v>30.434</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.7413</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:4">
+      <c r="A15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="5">
+        <v>393</v>
+      </c>
+      <c r="C15" s="6">
+        <v>34.303</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.7252</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:4">
+      <c r="A16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="5">
+        <v>327</v>
+      </c>
+      <c r="C16" s="6">
+        <v>39.285</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.7088</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" ht="14.25" spans="1:4">
+      <c r="A18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" ht="15" spans="1:4">
+      <c r="A19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5">
+        <v>654</v>
+      </c>
+      <c r="C19" s="5">
+        <v>22.19</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.7911</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:4">
+      <c r="A20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="5">
+        <v>589</v>
+      </c>
+      <c r="C20" s="5">
+        <v>22.19</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.7825</v>
+      </c>
+    </row>
+    <row r="21" ht="15" spans="1:4">
+      <c r="A21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="5">
+        <v>524</v>
+      </c>
+      <c r="C21" s="5">
+        <v>24.037</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.7702</v>
+      </c>
+    </row>
+    <row r="22" ht="15" spans="1:4">
+      <c r="A22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="5">
+        <v>458</v>
+      </c>
+      <c r="C22" s="5">
+        <v>26.181</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.7617</v>
+      </c>
+    </row>
+    <row r="23" ht="15" spans="1:4">
+      <c r="A23" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="5">
+        <v>393</v>
+      </c>
+      <c r="C23" s="5">
+        <v>27.732</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.7419</v>
+      </c>
+    </row>
+    <row r="24" ht="15" spans="1:4">
+      <c r="A24" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="7">
+        <v>327</v>
+      </c>
+      <c r="C24" s="4">
+        <v>31.88</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.7102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="8"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="8"/>
+      <c r="E27" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A17:D17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>